<commit_message>
#67, #71 - refactoring of IDataProvider and appropriate changes
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-demo/src/main/resources/excel/DsLookup/DsLookup.xlsx
+++ b/calculation-engine/engine-demo/src/main/resources/excel/DsLookup/DsLookup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="2805" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -415,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +521,13 @@
         <v>19</v>
       </c>
       <c r="F7" t="e">
-        <f ca="1">DSLOOKUP("Sheet1", "Family", "Smith", "Age" )</f>
+        <f ca="1">INDEX(DSLOOKUP("Sheet1", "Family", "Smith", "Age" ),1)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" t="e">
+        <f ca="1">INDEX(DSLOOKUP("Sheet1", "Family", "Smith", "Age" ),2)</f>
         <v>#NAME?</v>
       </c>
     </row>

</xml_diff>